<commit_message>
Added Test case ValidateSidebar
</commit_message>
<xml_diff>
--- a/SwagLabs/TestData/data.xlsx
+++ b/SwagLabs/TestData/data.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,12 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>secret_sauce</t>
   </si>
   <si>
     <t>standard_user</t>
+  </si>
+  <si>
+    <t>All Items</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Reset App State</t>
   </si>
 </sst>
 </file>
@@ -351,7 +364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -373,4 +386,43 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test case validate social media links
</commit_message>
<xml_diff>
--- a/SwagLabs/TestData/data.xlsx
+++ b/SwagLabs/TestData/data.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="4260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>secret_sauce</t>
   </si>
@@ -38,6 +40,15 @@
   </si>
   <si>
     <t>Reset App State</t>
+  </si>
+  <si>
+    <t>Sign In | LinkedIn</t>
+  </si>
+  <si>
+    <t>Sauce Labs - Home</t>
+  </si>
+  <si>
+    <t>Twitter</t>
   </si>
 </sst>
 </file>
@@ -392,7 +403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -425,4 +436,38 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>